<commit_message>
DONE! Now for review...
</commit_message>
<xml_diff>
--- a/documentation/Timesheets/Timesheet Gareth Stephenson.xlsx
+++ b/documentation/Timesheets/Timesheet Gareth Stephenson.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ELEN7046\ELEN7046_Group2_2016\documentation\Timesheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ELEN7046_Group2_2016\documentation\Timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Gareth Stephenson" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -120,12 +120,24 @@
   </si>
   <si>
     <t>Moving away from Apache SparkSQL, trying to use object based map reduce</t>
+  </si>
+  <si>
+    <t>Got CategoryCountPerHour program to use object based map reduce</t>
+  </si>
+  <si>
+    <t>Working on CategoryCountPerDay program</t>
+  </si>
+  <si>
+    <t>Group Presentation</t>
+  </si>
+  <si>
+    <t>Working on Group Report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
@@ -194,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -204,9 +216,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -391,23 +400,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -443,23 +435,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -612,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -624,20 +599,20 @@
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -655,7 +630,7 @@
       <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -675,7 +650,7 @@
       <c r="E3" s="6">
         <v>4</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <f>D3-C3</f>
         <v>0.16666666666666663</v>
       </c>
@@ -696,8 +671,8 @@
       <c r="E4" s="6">
         <v>6</v>
       </c>
-      <c r="F4" s="11">
-        <f t="shared" ref="F4:F68" si="0">D4-C4</f>
+      <c r="F4" s="10">
+        <f t="shared" ref="F4:F58" si="0">D4-C4</f>
         <v>0.25</v>
       </c>
     </row>
@@ -717,7 +692,7 @@
       <c r="E5" s="6">
         <v>2</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
@@ -738,7 +713,7 @@
       <c r="E6" s="6">
         <v>2</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f t="shared" si="0"/>
         <v>0.16666666666666674</v>
       </c>
@@ -759,7 +734,7 @@
       <c r="E7" s="6">
         <v>4</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <f t="shared" si="0"/>
         <v>0.33333333333333337</v>
       </c>
@@ -780,7 +755,7 @@
       <c r="E8" s="6">
         <v>4</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f t="shared" si="0"/>
         <v>0.20833333333333337</v>
       </c>
@@ -801,7 +776,7 @@
       <c r="E9" s="6">
         <v>4</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <f t="shared" si="0"/>
         <v>0.20833333333333337</v>
       </c>
@@ -822,7 +797,7 @@
       <c r="E10" s="6">
         <v>2</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
@@ -843,7 +818,7 @@
       <c r="E11" s="6">
         <v>3</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
@@ -864,7 +839,7 @@
       <c r="E12" s="6">
         <v>3</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
@@ -885,7 +860,7 @@
       <c r="E13" s="6">
         <v>2</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="10">
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
@@ -906,7 +881,7 @@
       <c r="E14" s="6">
         <v>3</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
@@ -927,7 +902,7 @@
       <c r="E15" s="6">
         <v>3</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="10">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
@@ -948,7 +923,7 @@
       <c r="E16" s="6">
         <v>8</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <f t="shared" si="0"/>
         <v>0.49999999999999994</v>
       </c>
@@ -969,7 +944,7 @@
       <c r="E17" s="6">
         <v>2</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
@@ -990,7 +965,7 @@
       <c r="E18" s="6">
         <v>4</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
@@ -1011,7 +986,7 @@
       <c r="E19" s="6">
         <v>4</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <f t="shared" si="0"/>
         <v>0.20833333333333337</v>
       </c>
@@ -1032,7 +1007,7 @@
       <c r="E20" s="6">
         <v>2</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="10">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
@@ -1053,7 +1028,7 @@
       <c r="E21" s="6">
         <v>4</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="10">
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
@@ -1074,7 +1049,7 @@
       <c r="E22" s="6">
         <v>5</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="10">
         <f t="shared" si="0"/>
         <v>0.20833333333333337</v>
       </c>
@@ -1095,7 +1070,7 @@
       <c r="E23" s="6">
         <v>8</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="10">
         <f t="shared" si="0"/>
         <v>0.49999999999999994</v>
       </c>
@@ -1116,7 +1091,7 @@
       <c r="E24" s="6">
         <v>2</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="10">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
@@ -1137,7 +1112,7 @@
       <c r="E25" s="6">
         <v>3</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="10">
         <f t="shared" si="0"/>
         <v>0.20833333333333337</v>
       </c>
@@ -1158,7 +1133,7 @@
       <c r="E26" s="6">
         <v>3</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="10">
         <f t="shared" si="0"/>
         <v>0.20833333333333337</v>
       </c>
@@ -1179,7 +1154,7 @@
       <c r="E27" s="6">
         <v>9</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F27" s="10">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
@@ -1200,7 +1175,7 @@
       <c r="E28" s="6">
         <v>2</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="10">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
@@ -1221,7 +1196,7 @@
       <c r="E29" s="6">
         <v>2</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="10">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
@@ -1231,20 +1206,20 @@
         <v>31</v>
       </c>
       <c r="B30" s="3">
-        <v>42514</v>
+        <v>42518</v>
       </c>
       <c r="C30" s="4">
-        <v>0.75</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D30" s="4">
-        <v>0.83333333333333337</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="E30" s="6">
-        <v>2</v>
-      </c>
-      <c r="F30" s="11">
-        <f t="shared" si="0"/>
-        <v>8.333333333333337E-2</v>
+        <v>4</v>
+      </c>
+      <c r="F30" s="10">
+        <f t="shared" si="0"/>
+        <v>0.49999999999999994</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1252,581 +1227,570 @@
         <v>31</v>
       </c>
       <c r="B31" s="3">
-        <v>42515</v>
+        <v>42519</v>
       </c>
       <c r="C31" s="4">
-        <v>0.875</v>
+        <v>0.5</v>
       </c>
       <c r="D31" s="4">
-        <v>0.91666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E31" s="6">
-        <v>1</v>
-      </c>
-      <c r="F31" s="11">
-        <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
+        <v>4</v>
+      </c>
+      <c r="F31" s="10">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333337</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="B32" s="3">
-        <v>42516</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42520</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E32" s="6">
+        <v>2</v>
+      </c>
+      <c r="F32" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
+      <c r="A33" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="B33" s="3">
-        <v>42517</v>
-      </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42521</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E33" s="6">
+        <v>2</v>
+      </c>
+      <c r="F33" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="B34" s="3">
-        <v>42518</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42523</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E34" s="6">
+        <v>2</v>
+      </c>
+      <c r="F34" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
+      <c r="A35" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B35" s="3">
-        <v>42519</v>
-      </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42526</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="E35" s="6">
+        <v>2</v>
+      </c>
+      <c r="F35" s="10">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B36" s="3">
-        <v>42520</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42528</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E36" s="6">
+        <v>2</v>
+      </c>
+      <c r="F36" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
+      <c r="A37" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B37" s="3">
-        <v>42521</v>
+        <v>42529</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="11">
+      <c r="F37" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
+      <c r="A38" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B38" s="3">
-        <v>42522</v>
-      </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42530</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E38" s="6">
+        <v>2</v>
+      </c>
+      <c r="F38" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
+      <c r="A39" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B39" s="3">
-        <v>42523</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42531</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E39" s="6">
+        <v>2</v>
+      </c>
+      <c r="F39" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
+      <c r="A40" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B40" s="3">
-        <v>42524</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42532</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E40" s="6">
+        <v>2</v>
+      </c>
+      <c r="F40" s="10">
+        <f t="shared" si="0"/>
+        <v>0.37499999999999994</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
+      <c r="A41" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="B41" s="3">
-        <v>42525</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42533</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E41" s="6">
+        <v>2</v>
+      </c>
+      <c r="F41" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B42" s="3">
-        <v>42526</v>
+        <v>42534</v>
       </c>
       <c r="C42" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E42" s="6">
+        <v>2</v>
+      </c>
+      <c r="F42" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="3">
+        <v>42535</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E43" s="6">
+        <v>2</v>
+      </c>
+      <c r="F43" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="3">
+        <v>42537</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E44" s="6">
+        <v>2</v>
+      </c>
+      <c r="F44" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="3">
+        <v>42538</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E45" s="6">
+        <v>2</v>
+      </c>
+      <c r="F45" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="3">
+        <v>42539</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="E46" s="6">
+        <v>8</v>
+      </c>
+      <c r="F46" s="10">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="D42" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="E42" s="6">
-        <v>2</v>
-      </c>
-      <c r="F42" s="11">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="3">
-        <v>42527</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3">
-        <v>42528</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="3">
-        <v>42529</v>
-      </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="3">
-        <v>42530</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
+      <c r="A47" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B47" s="3">
-        <v>42531</v>
-      </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42540</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E47" s="6">
+        <v>2</v>
+      </c>
+      <c r="F47" s="10">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666663</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B48" s="3">
-        <v>42532</v>
+        <v>42541</v>
       </c>
       <c r="C48" s="4">
-        <v>0.41666666666666669</v>
+        <v>0.75</v>
       </c>
       <c r="D48" s="4">
-        <v>0.79166666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E48" s="6">
         <v>2</v>
       </c>
-      <c r="F48" s="11">
-        <f t="shared" si="0"/>
-        <v>0.37499999999999994</v>
+      <c r="F48" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
+      <c r="A49" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="B49" s="3">
-        <v>42533</v>
-      </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42542</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E49" s="6">
+        <v>2</v>
+      </c>
+      <c r="F49" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
+      <c r="A50" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="B50" s="3">
-        <v>42534</v>
+        <v>42543</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="6"/>
-      <c r="F50" s="11">
+      <c r="F50" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
+      <c r="A51" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="B51" s="3">
-        <v>42535</v>
-      </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42544</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E51" s="6">
+        <v>2</v>
+      </c>
+      <c r="F51" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
+      <c r="A52" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="B52" s="3">
-        <v>42536</v>
-      </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42545</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E52" s="6">
+        <v>2</v>
+      </c>
+      <c r="F52" s="10">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
+      <c r="A53" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="B53" s="3">
-        <v>42537</v>
-      </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42547</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E53" s="6">
+        <v>2</v>
+      </c>
+      <c r="F53" s="10">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
+      <c r="A54" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B54" s="3">
-        <v>42538</v>
+        <v>42548</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="6"/>
-      <c r="F54" s="11">
+      <c r="F54" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B55" s="3">
-        <v>42539</v>
-      </c>
-      <c r="C55" s="4">
-        <v>0.375</v>
-      </c>
-      <c r="D55" s="4">
-        <v>0.875</v>
-      </c>
-      <c r="E55" s="6">
-        <v>8</v>
-      </c>
-      <c r="F55" s="11">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>42549</v>
+      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B56" s="3">
-        <v>42540</v>
-      </c>
-      <c r="C56" s="4">
-        <v>0.375</v>
-      </c>
-      <c r="D56" s="4">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="E56" s="6">
-        <v>2</v>
-      </c>
-      <c r="F56" s="11">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666663</v>
+        <v>42550</v>
+      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
+      <c r="A57" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="B57" s="3">
-        <v>42541</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>42551</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E57" s="6">
+        <v>1</v>
+      </c>
+      <c r="F57" s="10">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
+      <c r="A58" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="B58" s="3">
-        <v>42542</v>
-      </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
-      <c r="B59" s="3">
-        <v>42543</v>
-      </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="6"/>
+        <v>42552</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E58" s="6">
+        <v>8</v>
+      </c>
+      <c r="F58" s="10">
+        <f t="shared" si="0"/>
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E59" s="7">
+        <f>SUM(E3:E58)</f>
+        <v>163</v>
+      </c>
       <c r="F59" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
-      <c r="B60" s="3">
-        <v>42544</v>
-      </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
-      <c r="B61" s="3">
-        <v>42545</v>
-      </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
-      <c r="B62" s="3">
-        <v>42546</v>
-      </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B63" s="3">
-        <v>42547</v>
-      </c>
-      <c r="C63" s="4">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="D63" s="4">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="E63" s="6">
-        <v>2</v>
-      </c>
-      <c r="F63" s="11">
-        <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
-      <c r="B64" s="3">
-        <v>42548</v>
-      </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
-      <c r="B65" s="3">
-        <v>42549</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
-      <c r="B66" s="3">
-        <v>42550</v>
-      </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="3">
-        <v>42551</v>
-      </c>
-      <c r="C67" s="4">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="D67" s="4">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E67" s="6">
-        <v>1</v>
-      </c>
-      <c r="F67" s="11">
-        <f t="shared" si="0"/>
-        <v>6.25E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B68" s="3">
-        <v>42552</v>
-      </c>
-      <c r="C68" s="4">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D68" s="4">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E68" s="6">
-        <v>8</v>
-      </c>
-      <c r="F68" s="11">
-        <f t="shared" si="0"/>
-        <v>0.29166666666666669</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="2"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="11">
-        <f t="shared" ref="F69" si="1">D69-C69</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E70" s="8">
-        <f>SUM(E3:E69)</f>
-        <v>128</v>
-      </c>
-      <c r="F70" s="12">
-        <f>SUM(F5:F69)</f>
-        <v>6.604166666666667</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+        <f>SUM(F5:F58)</f>
+        <v>8.5624999999999947</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>

</xml_diff>